<commit_message>
Update before implementing new Spinney Calcs. Added in new narrow CDF files.
</commit_message>
<xml_diff>
--- a/ElectroCalcs/ElectroCalcs.xlsx
+++ b/ElectroCalcs/ElectroCalcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\OneDrive\Documents\ASE6002\ModelProject\ElectroCalcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CD116B4-AF64-4DE9-B06F-4CC794A32203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F49E5B-4BF5-4650-A42C-88244D7834E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{88B280C3-4562-4D67-9373-B80D3F289D5B}"/>
   </bookViews>

</xml_diff>

<commit_message>
Model after doing Evolve run and dealing with OneDrive shenanigans.
</commit_message>
<xml_diff>
--- a/ElectroCalcs/ElectroCalcs.xlsx
+++ b/ElectroCalcs/ElectroCalcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eba1ba43692f98ec/Documents/ASE6002/ModelProject/ElectroCalcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CD116B4-AF64-4DE9-B06F-4CC794A32203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19287" documentId="13_ncr:1_{C8F49E5B-4BF5-4650-A42C-88244D7834E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA12C214-1356-478A-998D-0C093EC24EC5}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{88B280C3-4562-4D67-9373-B80D3F289D5B}"/>
   </bookViews>
@@ -500,7 +500,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>0.3</v>
+        <v>0.93720000000000003</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -510,7 +510,7 @@
       </c>
       <c r="E2">
         <f>1.931*B2+0.2579</f>
-        <v>0.83720000000000006</v>
+        <v>2.0676332000000004</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="E3">
         <f>50.039*B2+18.089</f>
-        <v>33.100699999999996</v>
+        <v>64.985550799999999</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -567,7 +567,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>11.990399999999999</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -577,7 +577,7 @@
       </c>
       <c r="E2">
         <f>B$2*G2+H2</f>
-        <v>0.76380000000000003</v>
+        <v>1.6201239999999999</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -595,7 +595,7 @@
       </c>
       <c r="E3">
         <f>B$2*G3+H3</f>
-        <v>160.12299999999999</v>
+        <v>297.64513919999996</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -663,7 +663,7 @@
       </c>
       <c r="E9">
         <f>AVERAGE(E2,E5)</f>
-        <v>0.93025000000000002</v>
+        <v>1.358412</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -675,7 +675,7 @@
       </c>
       <c r="E10">
         <f>AVERAGE(E3,E6)</f>
-        <v>184.7739</v>
+        <v>253.53496959999998</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Spinney and Matt updates and LHS implemented.
</commit_message>
<xml_diff>
--- a/ElectroCalcs/ElectroCalcs.xlsx
+++ b/ElectroCalcs/ElectroCalcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eba1ba43692f98ec/Documents/ASE6002/ModelProject/ElectroCalcs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dspin\iCloudDrive\GT PMASE\ASE6002\TA-4\ASE6002_Model-main_112624\ASE6002_Model-main\ElectroCalcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19287" documentId="13_ncr:1_{C8F49E5B-4BF5-4650-A42C-88244D7834E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA12C214-1356-478A-998D-0C093EC24EC5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102CD091-A0D4-4BF4-B32C-582839BBEE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{88B280C3-4562-4D67-9373-B80D3F289D5B}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{88B280C3-4562-4D67-9373-B80D3F289D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="motorCalcs" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Inputs</t>
   </si>
@@ -104,14 +104,99 @@
   </si>
   <si>
     <t>motorPrice</t>
+  </si>
+  <si>
+    <r>
+      <t>6.6303x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 31.91x + 170.05</t>
+    </r>
+  </si>
+  <si>
+    <t>BatteryCost</t>
+  </si>
+  <si>
+    <r>
+      <t>y = -0.0355x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 0.7489x + 0.3598</t>
+    </r>
+  </si>
+  <si>
+    <t>BatteryWeight</t>
+  </si>
+  <si>
+    <r>
+      <t>= 1.2097x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.5862</t>
+    </r>
+  </si>
+  <si>
+    <t>0.3424x + 1.3273</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -477,17 +562,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832A2C58-70FF-46DC-9BE6-09008E951CF6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -495,12 +580,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2">
-        <v>0.93720000000000003</v>
+        <v>1.002</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -510,19 +595,19 @@
       </c>
       <c r="E2">
         <f>1.931*B2+0.2579</f>
-        <v>2.0676332000000004</v>
+        <v>2.1927620000000001</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3">
         <f>50.039*B2+18.089</f>
-        <v>64.985550799999999</v>
+        <v>68.228078000000011</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -535,20 +620,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C1AB6D-5338-4176-A91C-31BBF0F91FB4}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,13 +647,20 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1">
+        <f>(J3*B2^2)+(J4*B2)+J5</f>
+        <v>740.49461306630019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>11.990399999999999</v>
+        <v>11.989000000000001</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -577,7 +670,7 @@
       </c>
       <c r="E2">
         <f>B$2*G2+H2</f>
-        <v>1.6201239999999999</v>
+        <v>1.6199525000000001</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -589,13 +682,13 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3">
         <f>B$2*G3+H3</f>
-        <v>297.64513919999996</v>
+        <v>297.61759699999999</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -606,8 +699,19 @@
       <c r="H3">
         <v>61.758000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <v>6.6303000000000001</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>-31.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -633,8 +737,11 @@
       <c r="H5">
         <v>0.2147</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="J5">
+        <v>170.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>8</v>
       </c>
@@ -652,33 +759,93 @@
         <v>78.841999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8">
+        <f>J14*B2^J15</f>
+        <v>5.1887201972974824</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9">
-        <f>AVERAGE(E2,E5)</f>
-        <v>1.358412</v>
+        <f>L16/2.2</f>
+        <v>4.2070696134615417</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="J9">
+        <v>-3.5499999999999997E-2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10">
-        <f>AVERAGE(E3,E6)</f>
-        <v>253.53496959999998</v>
+        <f>L1</f>
+        <v>740.49461306630019</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
+      </c>
+      <c r="J10">
+        <v>0.74890000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>0.35980000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>1.2097</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>0.58620000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16">
+        <f>J18*B2^J19</f>
+        <v>9.2555531496153929</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>0.34239999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>1.3272999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +859,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>